<commit_message>
refatorando o consolidador para modelo ETL
</commit_message>
<xml_diff>
--- a/app/data/absenteeism_data_0.xlsx
+++ b/app/data/absenteeism_data_0.xlsx
@@ -476,103 +476,103 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>31287</v>
+        <v>2727</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dra. Milena Fernandes</t>
+          <t>Emanuella Gonçalves</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Recursos Humanos</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Viagem de negócios</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45089</v>
+        <v>45092</v>
       </c>
       <c r="G2" t="n">
-        <v>2999.42</v>
+        <v>10077.26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>74040</v>
+        <v>77844</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Leonardo Viana</t>
+          <t>Samuel Moreira</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Operações</t>
+          <t>Recursos Humanos</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Doença</t>
+          <t>Viagem de negócios</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45100</v>
+        <v>45081</v>
       </c>
       <c r="G3" t="n">
-        <v>11777.21</v>
+        <v>6297.91</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>74585</v>
+        <v>38990</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Maria Vitória da Cunha</t>
+          <t>Juliana das Neves</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Vendas</t>
+          <t>Atendimento ao Cliente</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Viagem de negócios</t>
+          <t>Consulta médica</t>
         </is>
       </c>
       <c r="E4" t="n">
         <v>6</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45100</v>
+        <v>45102</v>
       </c>
       <c r="G4" t="n">
-        <v>5440.68</v>
+        <v>10889.64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>24322</v>
+        <v>91830</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cecília Campos</t>
+          <t>Lorena Moura</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Financeiro</t>
+          <t>P&amp;D</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -581,85 +581,85 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45082</v>
+        <v>45099</v>
       </c>
       <c r="G5" t="n">
-        <v>7708.75</v>
+        <v>11922.9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>48339</v>
+        <v>22631</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sabrina da Mata</t>
+          <t>Alice Souza</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Vendas</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Viagem de negócios</t>
+          <t>Doença</t>
         </is>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45079</v>
+        <v>45095</v>
       </c>
       <c r="G6" t="n">
-        <v>3397.38</v>
+        <v>8721.92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>30971</v>
+        <v>32392</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bruna da Costa</t>
+          <t>Giovanna da Cunha</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Financeiro</t>
+          <t>Atendimento ao Cliente</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Problemas pessoais</t>
+          <t>Viagem de negócios</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45082</v>
+        <v>45083</v>
       </c>
       <c r="G7" t="n">
-        <v>10985.96</v>
+        <v>2738.37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7603</v>
+        <v>12967</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>João Gabriel Oliveira</t>
+          <t>Brenda Ferreira</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Atendimento ao Cliente</t>
+          <t>Financeiro</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45085</v>
+        <v>45086</v>
       </c>
       <c r="G8" t="n">
-        <v>7832.45</v>
+        <v>6341.91</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>73015</v>
+        <v>48251</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Luiza da Rosa</t>
+          <t>Joaquim Campos</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -697,71 +697,71 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45078</v>
+        <v>45095</v>
       </c>
       <c r="G9" t="n">
-        <v>6523.39</v>
+        <v>12194.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>96459</v>
+        <v>39378</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Pedro Henrique Ferreira</t>
+          <t>Luiz Otávio Nogueira</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Engenharia</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Viagem de negócios</t>
+          <t>Consulta médica</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45100</v>
+        <v>45087</v>
       </c>
       <c r="G10" t="n">
-        <v>9508.76</v>
+        <v>8490.700000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>74973</v>
+        <v>92452</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rafaela Cunha</t>
+          <t>Alexandre Duarte</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Vendas</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Viagem de negócios</t>
+          <t>Consulta médica</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45088</v>
+        <v>45092</v>
       </c>
       <c r="G11" t="n">
-        <v>7790.53</v>
+        <v>4987.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>